<commit_message>
updates of parsing fine-design, zwilling
</commit_message>
<xml_diff>
--- a/src/files/meta/xml-list/xml-list.xlsx
+++ b/src/files/meta/xml-list/xml-list.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\kitchen-time\crawler\dist\files\meta\xml-list\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\kitchen-time\crawler\src\files\meta\xml-list\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27870" windowHeight="13020"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
@@ -80,9 +86,6 @@
     <t>Лимарс</t>
   </si>
   <si>
-    <t>https://limars.ru/partners.xml</t>
-  </si>
-  <si>
     <t>COLDVINE</t>
   </si>
   <si>
@@ -236,59 +239,71 @@
     <t>http://194.186.103.234:27705/api/v1/yml/file_standard</t>
   </si>
   <si>
+    <t>Zwilling</t>
+  </si>
+  <si>
+    <t>ftp://ftp2.pmkc.ru/</t>
+  </si>
+  <si>
+    <t>Anna Lafarg</t>
+  </si>
+  <si>
+    <t>https://www.fissler-shop.ru/u/annalafarg.xml</t>
+  </si>
+  <si>
+    <t>EASY LIFE</t>
+  </si>
+  <si>
+    <t>FISSLER</t>
+  </si>
+  <si>
+    <t>JULIA VYSOTSKAYA</t>
+  </si>
+  <si>
+    <t>MAXWELL &amp; WILLIAMS</t>
+  </si>
+  <si>
+    <t>ANNA LAFARG</t>
+  </si>
+  <si>
+    <t>EOF</t>
+  </si>
+  <si>
     <t>NADOBA</t>
   </si>
   <si>
-    <t>Zwilling</t>
-  </si>
-  <si>
-    <t>ftp://ftp2.pmkc.ru/</t>
-  </si>
-  <si>
     <t>BALLARINI</t>
   </si>
   <si>
+    <t>BSF</t>
+  </si>
+  <si>
+    <t>STAUB</t>
+  </si>
+  <si>
     <t>ZWILLING</t>
   </si>
   <si>
-    <t>BSF</t>
-  </si>
-  <si>
-    <t>STAUB</t>
-  </si>
-  <si>
-    <t>Anna Lafarg</t>
-  </si>
-  <si>
-    <t>https://www.fissler-shop.ru/u/annalafarg.xml</t>
-  </si>
-  <si>
-    <t>EASY LIFE</t>
-  </si>
-  <si>
-    <t>FISSLER</t>
-  </si>
-  <si>
-    <t>JULIA VYSOTSKAYA</t>
-  </si>
-  <si>
-    <t>MAXWELL &amp; WILLIAMS</t>
-  </si>
-  <si>
-    <t>ANNA LAFARG</t>
-  </si>
-  <si>
-    <t>EOF</t>
+    <t>https://limars.ru/index.php?route=feed/ocext_feed_generator_yamarket&amp;token=73414</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -327,16 +342,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -617,8 +635,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D500"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A490" workbookViewId="0">
-      <selection activeCell="B504" sqref="B504"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -733,14 +751,14 @@
       <c r="A12" t="s">
         <v>17</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" t="s">
         <v>18</v>
-      </c>
-      <c r="C12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -748,7 +766,7 @@
         <v>6</v>
       </c>
       <c r="D13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -756,7 +774,7 @@
         <v>6</v>
       </c>
       <c r="D14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -764,21 +782,21 @@
         <v>6</v>
       </c>
       <c r="D15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" t="s">
         <v>23</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" t="s">
         <v>24</v>
-      </c>
-      <c r="C16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -786,7 +804,7 @@
         <v>6</v>
       </c>
       <c r="D17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -794,21 +812,21 @@
         <v>6</v>
       </c>
       <c r="D18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" t="s">
         <v>28</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" t="s">
         <v>29</v>
-      </c>
-      <c r="C19" t="s">
-        <v>6</v>
-      </c>
-      <c r="D19" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -816,7 +834,7 @@
         <v>6</v>
       </c>
       <c r="D20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -824,7 +842,7 @@
         <v>6</v>
       </c>
       <c r="D21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -832,7 +850,7 @@
         <v>6</v>
       </c>
       <c r="D22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -840,7 +858,7 @@
         <v>6</v>
       </c>
       <c r="D23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -848,7 +866,7 @@
         <v>6</v>
       </c>
       <c r="D24" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -856,7 +874,7 @@
         <v>6</v>
       </c>
       <c r="D25" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -864,7 +882,7 @@
         <v>6</v>
       </c>
       <c r="D26" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -872,7 +890,7 @@
         <v>6</v>
       </c>
       <c r="D27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -880,7 +898,7 @@
         <v>6</v>
       </c>
       <c r="D28" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -888,7 +906,7 @@
         <v>6</v>
       </c>
       <c r="D29" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -896,7 +914,7 @@
         <v>6</v>
       </c>
       <c r="D30" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -904,7 +922,7 @@
         <v>6</v>
       </c>
       <c r="D31" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -912,7 +930,7 @@
         <v>6</v>
       </c>
       <c r="D32" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -920,7 +938,7 @@
         <v>6</v>
       </c>
       <c r="D33" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -928,35 +946,35 @@
         <v>6</v>
       </c>
       <c r="D34" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>45</v>
+      </c>
+      <c r="B35" t="s">
         <v>46</v>
       </c>
-      <c r="B35" t="s">
+      <c r="C35" t="s">
+        <v>6</v>
+      </c>
+      <c r="D35" t="s">
         <v>47</v>
-      </c>
-      <c r="C35" t="s">
-        <v>6</v>
-      </c>
-      <c r="D35" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>48</v>
+      </c>
+      <c r="B36" t="s">
         <v>49</v>
       </c>
-      <c r="B36" t="s">
+      <c r="C36" t="s">
+        <v>6</v>
+      </c>
+      <c r="D36" t="s">
         <v>50</v>
-      </c>
-      <c r="C36" t="s">
-        <v>6</v>
-      </c>
-      <c r="D36" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -964,7 +982,7 @@
         <v>6</v>
       </c>
       <c r="D37" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -972,7 +990,7 @@
         <v>6</v>
       </c>
       <c r="D38" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -980,7 +998,7 @@
         <v>6</v>
       </c>
       <c r="D39" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -988,21 +1006,21 @@
         <v>6</v>
       </c>
       <c r="D40" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>55</v>
+      </c>
+      <c r="B41" t="s">
         <v>56</v>
       </c>
-      <c r="B41" t="s">
+      <c r="C41" t="s">
+        <v>6</v>
+      </c>
+      <c r="D41" t="s">
         <v>57</v>
-      </c>
-      <c r="C41" t="s">
-        <v>6</v>
-      </c>
-      <c r="D41" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -1010,7 +1028,7 @@
         <v>6</v>
       </c>
       <c r="D42" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -1018,7 +1036,7 @@
         <v>6</v>
       </c>
       <c r="D43" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -1026,7 +1044,7 @@
         <v>6</v>
       </c>
       <c r="D44" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -1034,7 +1052,7 @@
         <v>6</v>
       </c>
       <c r="D45" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -1042,7 +1060,7 @@
         <v>6</v>
       </c>
       <c r="D46" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -1050,7 +1068,7 @@
         <v>6</v>
       </c>
       <c r="D47" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -1058,7 +1076,7 @@
         <v>6</v>
       </c>
       <c r="D48" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -1066,7 +1084,7 @@
         <v>6</v>
       </c>
       <c r="D49" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -1074,35 +1092,29 @@
         <v>6</v>
       </c>
       <c r="D50" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B51" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C51" t="s">
         <v>6</v>
       </c>
       <c r="D51" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>71</v>
-      </c>
-      <c r="B52" t="s">
-        <v>72</v>
-      </c>
       <c r="C52" t="s">
         <v>6</v>
       </c>
       <c r="D52" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -1110,7 +1122,7 @@
         <v>6</v>
       </c>
       <c r="D53" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -1118,29 +1130,35 @@
         <v>6</v>
       </c>
       <c r="D54" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>67</v>
+      </c>
+      <c r="B55" t="s">
+        <v>68</v>
+      </c>
       <c r="C55" t="s">
         <v>6</v>
       </c>
       <c r="D55" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B56" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="C56" t="s">
         <v>6</v>
       </c>
       <c r="D56" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -1148,7 +1166,7 @@
         <v>6</v>
       </c>
       <c r="D57" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -1156,7 +1174,7 @@
         <v>6</v>
       </c>
       <c r="D58" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -1164,7 +1182,7 @@
         <v>6</v>
       </c>
       <c r="D59" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -1172,12 +1190,12 @@
         <v>6</v>
       </c>
       <c r="D60" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
     </row>
     <row r="500" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A500" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -1188,8 +1206,8 @@
     <hyperlink ref="B35" r:id="rId4"/>
     <hyperlink ref="B36" r:id="rId5"/>
     <hyperlink ref="B41" r:id="rId6"/>
-    <hyperlink ref="B51" r:id="rId7"/>
-    <hyperlink ref="B52" r:id="rId8"/>
+    <hyperlink ref="B55" r:id="rId7"/>
+    <hyperlink ref="B51" r:id="rId8"/>
     <hyperlink ref="B56" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added addwine and small fixes of zwilling
</commit_message>
<xml_diff>
--- a/src/files/meta/xml-list/xml-list.xlsx
+++ b/src/files/meta/xml-list/xml-list.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="96">
   <si>
     <t>Поставщик</t>
   </si>
@@ -285,13 +285,46 @@
   </si>
   <si>
     <t>https://limars.ru/index.php?route=feed/ocext_feed_generator_yamarket&amp;token=73414</t>
+  </si>
+  <si>
+    <t>https://sellers.addwine.ru/api/v1/products/yml?key=d217a657-26c4-449b-ae09-e276490a6561</t>
+  </si>
+  <si>
+    <t>CORAVIN</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LAGUIOLE</t>
+  </si>
+  <si>
+    <t>ITALESSE</t>
+  </si>
+  <si>
+    <t>SOPHIENWALD</t>
+  </si>
+  <si>
+    <t>THE DURAND</t>
+  </si>
+  <si>
+    <t>WINESAVE</t>
+  </si>
+  <si>
+    <t>ZALTO</t>
+  </si>
+  <si>
+    <t>SYDONIOS</t>
+  </si>
+  <si>
+    <t>MARK THOMAS</t>
+  </si>
+  <si>
+    <t>Addwine</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -304,6 +337,21 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -333,9 +381,7 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -346,18 +392,107 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="8">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -368,6 +503,19 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Таблица2" displayName="Таблица2" ref="A1:D69" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4">
+  <autoFilter ref="A1:D69"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="Поставщик" dataDxfId="3"/>
+    <tableColumn id="2" name="Ссылка на XML" dataDxfId="2"/>
+    <tableColumn id="3" name="Формат обновления" dataDxfId="1"/>
+    <tableColumn id="4" name="Бренд" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -635,15 +783,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D500"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.5703125" customWidth="1"/>
     <col min="2" max="2" width="84.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" customWidth="1"/>
     <col min="4" max="4" width="25.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -662,535 +810,727 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="C2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="C12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="C12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" t="s">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C14" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" t="s">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C15" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15" t="s">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16" t="s">
+      <c r="C16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C17" t="s">
-        <v>6</v>
-      </c>
-      <c r="D17" t="s">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C18" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18" t="s">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="A19" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C19" t="s">
-        <v>6</v>
-      </c>
-      <c r="D19" t="s">
+      <c r="C19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C20" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20" t="s">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C21" t="s">
-        <v>6</v>
-      </c>
-      <c r="D21" t="s">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C22" t="s">
-        <v>6</v>
-      </c>
-      <c r="D22" t="s">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C23" t="s">
-        <v>6</v>
-      </c>
-      <c r="D23" t="s">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" s="2" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C24" t="s">
-        <v>6</v>
-      </c>
-      <c r="D24" t="s">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C25" t="s">
-        <v>6</v>
-      </c>
-      <c r="D25" t="s">
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" s="2" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C26" t="s">
-        <v>6</v>
-      </c>
-      <c r="D26" t="s">
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C27" t="s">
-        <v>6</v>
-      </c>
-      <c r="D27" t="s">
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27" s="2" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C28" t="s">
-        <v>6</v>
-      </c>
-      <c r="D28" t="s">
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28" s="2" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C29" t="s">
-        <v>6</v>
-      </c>
-      <c r="D29" t="s">
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" s="2" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C30" t="s">
-        <v>6</v>
-      </c>
-      <c r="D30" t="s">
+      <c r="A30" s="2"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" s="2" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C31" t="s">
-        <v>6</v>
-      </c>
-      <c r="D31" t="s">
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" s="2" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C32" t="s">
-        <v>6</v>
-      </c>
-      <c r="D32" t="s">
+      <c r="A32" s="2"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" s="2" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C33" t="s">
-        <v>6</v>
-      </c>
-      <c r="D33" t="s">
+      <c r="A33" s="2"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" s="2" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C34" t="s">
-        <v>6</v>
-      </c>
-      <c r="D34" t="s">
+      <c r="A34" s="2"/>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34" s="2" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="A35" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C35" t="s">
-        <v>6</v>
-      </c>
-      <c r="D35" t="s">
+      <c r="C35" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D35" s="2" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="A36" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C36" t="s">
-        <v>6</v>
-      </c>
-      <c r="D36" t="s">
+      <c r="C36" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D36" s="2" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C37" t="s">
-        <v>6</v>
-      </c>
-      <c r="D37" t="s">
+      <c r="A37" s="2"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D37" s="2" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C38" t="s">
-        <v>6</v>
-      </c>
-      <c r="D38" t="s">
+      <c r="A38" s="2"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D38" s="2" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C39" t="s">
-        <v>6</v>
-      </c>
-      <c r="D39" t="s">
+      <c r="A39" s="2"/>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D39" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C40" t="s">
-        <v>6</v>
-      </c>
-      <c r="D40" t="s">
+      <c r="A40" s="2"/>
+      <c r="B40" s="2"/>
+      <c r="C40" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D40" s="2" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+      <c r="A41" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C41" t="s">
-        <v>6</v>
-      </c>
-      <c r="D41" t="s">
+      <c r="C41" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D41" s="2" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C42" t="s">
-        <v>6</v>
-      </c>
-      <c r="D42" t="s">
+      <c r="A42" s="2"/>
+      <c r="B42" s="2"/>
+      <c r="C42" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D42" s="2" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C43" t="s">
-        <v>6</v>
-      </c>
-      <c r="D43" t="s">
+      <c r="A43" s="2"/>
+      <c r="B43" s="2"/>
+      <c r="C43" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D43" s="2" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C44" t="s">
-        <v>6</v>
-      </c>
-      <c r="D44" t="s">
+      <c r="A44" s="2"/>
+      <c r="B44" s="2"/>
+      <c r="C44" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D44" s="2" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C45" t="s">
-        <v>6</v>
-      </c>
-      <c r="D45" t="s">
+      <c r="A45" s="2"/>
+      <c r="B45" s="2"/>
+      <c r="C45" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D45" s="2" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C46" t="s">
-        <v>6</v>
-      </c>
-      <c r="D46" t="s">
+      <c r="A46" s="2"/>
+      <c r="B46" s="2"/>
+      <c r="C46" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D46" s="2" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C47" t="s">
-        <v>6</v>
-      </c>
-      <c r="D47" t="s">
+      <c r="A47" s="2"/>
+      <c r="B47" s="2"/>
+      <c r="C47" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D47" s="2" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C48" t="s">
-        <v>6</v>
-      </c>
-      <c r="D48" t="s">
+      <c r="A48" s="2"/>
+      <c r="B48" s="2"/>
+      <c r="C48" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D48" s="2" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C49" t="s">
-        <v>6</v>
-      </c>
-      <c r="D49" t="s">
+      <c r="A49" s="2"/>
+      <c r="B49" s="2"/>
+      <c r="C49" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D49" s="2" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C50" t="s">
-        <v>6</v>
-      </c>
-      <c r="D50" t="s">
+      <c r="A50" s="2"/>
+      <c r="B50" s="2"/>
+      <c r="C50" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D50" s="2" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+      <c r="A51" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B51" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C51" t="s">
-        <v>6</v>
-      </c>
-      <c r="D51" t="s">
+      <c r="C51" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D51" s="2" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C52" t="s">
-        <v>6</v>
-      </c>
-      <c r="D52" t="s">
+      <c r="A52" s="2"/>
+      <c r="B52" s="2"/>
+      <c r="C52" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D52" s="2" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C53" t="s">
-        <v>6</v>
-      </c>
-      <c r="D53" t="s">
+      <c r="A53" s="2"/>
+      <c r="B53" s="2"/>
+      <c r="C53" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D53" s="2" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C54" t="s">
-        <v>6</v>
-      </c>
-      <c r="D54" t="s">
+      <c r="A54" s="2"/>
+      <c r="B54" s="2"/>
+      <c r="C54" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D54" s="2" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+      <c r="A55" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B55" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C55" t="s">
-        <v>6</v>
-      </c>
-      <c r="D55" t="s">
+      <c r="C55" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D55" s="2" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+      <c r="A56" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B56" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C56" t="s">
-        <v>6</v>
-      </c>
-      <c r="D56" t="s">
+      <c r="C56" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D56" s="2" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C57" t="s">
-        <v>6</v>
-      </c>
-      <c r="D57" t="s">
+      <c r="A57" s="2"/>
+      <c r="B57" s="2"/>
+      <c r="C57" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D57" s="2" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C58" t="s">
-        <v>6</v>
-      </c>
-      <c r="D58" t="s">
+      <c r="A58" s="2"/>
+      <c r="B58" s="2"/>
+      <c r="C58" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D58" s="2" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C59" t="s">
-        <v>6</v>
-      </c>
-      <c r="D59" t="s">
+      <c r="A59" s="2"/>
+      <c r="B59" s="2"/>
+      <c r="C59" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D59" s="2" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C60" t="s">
-        <v>6</v>
-      </c>
-      <c r="D60" t="s">
+      <c r="A60" s="2"/>
+      <c r="B60" s="2"/>
+      <c r="C60" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D60" s="2" t="s">
         <v>77</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="2"/>
+      <c r="B62" s="2"/>
+      <c r="C62" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="2"/>
+      <c r="B63" s="2"/>
+      <c r="C63" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="2"/>
+      <c r="B64" s="2"/>
+      <c r="C64" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="2"/>
+      <c r="B65" s="2"/>
+      <c r="C65" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="2"/>
+      <c r="B66" s="2"/>
+      <c r="C66" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="2"/>
+      <c r="B67" s="2"/>
+      <c r="C67" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="2"/>
+      <c r="B68" s="2"/>
+      <c r="C68" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="2"/>
+      <c r="B69" s="2"/>
+      <c r="C69" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="500" spans="1:1" x14ac:dyDescent="0.25">
@@ -1211,5 +1551,9 @@
     <hyperlink ref="B56" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <tableParts count="1">
+    <tablePart r:id="rId10"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>